<commit_message>
fix 10.06.2025 Price 18h+22
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV_ver.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV_ver.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\ТЗ программа подбора TRV, RDT\ТЗ клапаны TRV\27.05.2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0558216-379E-4BA1-9A72-D4CB1E2878F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B18B201-2CAF-4040-836C-B3AC86B0A649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1665" windowWidth="12765" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -325,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -350,6 +350,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -360,55 +411,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,7 +757,7 @@
   <dimension ref="A1:W51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C5" sqref="C5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,17 +776,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -787,12 +796,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="26"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -810,16 +819,16 @@
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -834,19 +843,19 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -861,19 +870,19 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="32"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -888,12 +897,12 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -915,19 +924,19 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -942,17 +951,17 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="7"/>
       <c r="K8" s="4"/>
       <c r="L8" s="2"/>
@@ -969,17 +978,17 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
       <c r="J9" s="7"/>
       <c r="K9" s="6"/>
       <c r="L9" s="2"/>
@@ -996,17 +1005,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="7"/>
       <c r="K10" s="4" t="s">
         <v>16</v>
@@ -1025,20 +1034,20 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
       <c r="K11" s="4"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1054,13 +1063,13 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1081,19 +1090,19 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="15"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1108,19 +1117,19 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="15"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1160,21 +1169,21 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="9" t="s">
         <v>2</v>
       </c>
@@ -1201,13 +1210,13 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -1226,19 +1235,19 @@
       <c r="W17" s="2"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2042,15 +2051,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A8:I8"/>
     <mergeCell ref="C4:K4"/>
     <mergeCell ref="E13:K13"/>
     <mergeCell ref="E14:K14"/>
@@ -2062,13 +2062,22 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A8:I8"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A9:I9"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
   </mergeCells>

</xml_diff>

<commit_message>
fix 11.06.2025 price 18h + 25
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV_ver.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV_ver.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B18B201-2CAF-4040-836C-B3AC86B0A649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E90027D-F7B2-4E03-8F7B-92C39E147681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,57 +350,66 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -409,15 +418,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,23 +770,23 @@
     <col min="6" max="7" width="6.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="3" customWidth="1"/>
     <col min="12" max="23" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -796,12 +796,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -819,16 +819,16 @@
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -843,19 +843,19 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="32"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -870,19 +870,19 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="32"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -897,12 +897,12 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -924,19 +924,19 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -951,17 +951,17 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="14"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="7"/>
       <c r="K8" s="4"/>
       <c r="L8" s="2"/>
@@ -978,17 +978,17 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="7"/>
       <c r="K9" s="6"/>
       <c r="L9" s="2"/>
@@ -1005,17 +1005,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="7"/>
       <c r="K10" s="4" t="s">
         <v>16</v>
@@ -1034,20 +1034,20 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
       <c r="K11" s="4"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1063,13 +1063,13 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1090,19 +1090,19 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1117,19 +1117,19 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="21"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1169,21 +1169,21 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="27"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="29"/>
+      <c r="G16" s="32"/>
       <c r="H16" s="9" t="s">
         <v>2</v>
       </c>
@@ -1210,13 +1210,13 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="32"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -1235,19 +1235,19 @@
       <c r="W17" s="2"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2051,20 +2051,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="E13:K13"/>
-    <mergeCell ref="E14:K14"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A9:I9"/>
     <mergeCell ref="A18:K18"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A14:D14"/>
@@ -2080,6 +2066,20 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="E13:K13"/>
+    <mergeCell ref="E14:K14"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A9:I9"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>